<commit_message>
Update HOTAS Switch and Button - Quick Reference - BASIC.xlsx
Version correction
</commit_message>
<xml_diff>
--- a/Maps/HOTAS Switch and Button - Quick Reference - BASIC.xlsx
+++ b/Maps/HOTAS Switch and Button - Quick Reference - BASIC.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Den\OneDrive\Personal\Thrustmaster\TARGET\Clicker\Development\ED_TargetScript-502\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB12BC6F-BF59-41ED-A222-E0CA8709BAD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30465" windowHeight="14430"/>
+    <workbookView xWindow="6765" yWindow="960" windowWidth="28305" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -368,13 +369,13 @@
     <t>TargetNextHostileShip</t>
   </si>
   <si>
-    <t>HOTAS - Quick reference - v5.0.2 - BASIC</t>
+    <t>HOTAS - Quick reference - v5.02 - BASIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -743,48 +744,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -804,9 +799,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1156,11 +1148,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O80"/>
+  <dimension ref="B1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:O2"/>
@@ -1186,710 +1178,644 @@
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="41"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="37"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="37"/>
+      <c r="N2" s="37"/>
+      <c r="O2" s="38"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
-      <c r="G4" s="42" t="s">
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="41"/>
+      <c r="G4" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
-      <c r="L4" s="42" t="s">
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="41"/>
+      <c r="L4" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="44"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="41"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-    </row>
+    <row r="6" spans="2:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="G7" s="17" t="s">
+      <c r="E7" s="19"/>
+      <c r="G7" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24"/>
-      <c r="L7" s="16" t="s">
+      <c r="H7" s="12"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
+      <c r="L7" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="M7" s="21"/>
-      <c r="N7" s="21"/>
-      <c r="O7" s="22"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="25"/>
-      <c r="G8" s="31" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="22"/>
+      <c r="G8" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
-      <c r="L8" s="15" t="s">
+      <c r="H8" s="29"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="L8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="4"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="3"/>
     </row>
     <row r="9" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="38"/>
-      <c r="L9" s="19" t="s">
+      <c r="H9" s="33"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="35"/>
+      <c r="L9" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="28"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="G11" s="26" t="s">
+      <c r="B11" s="10"/>
+      <c r="G11" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27" t="s">
+      <c r="H11" s="24"/>
+      <c r="I11" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="J11" s="28"/>
-      <c r="L11" s="16" t="s">
+      <c r="J11" s="25"/>
+      <c r="L11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="M11" s="21"/>
-      <c r="N11" s="21" t="s">
+      <c r="M11" s="12"/>
+      <c r="N11" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="O11" s="22"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="28"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="L12" s="19" t="s">
+      <c r="E12" s="25"/>
+      <c r="G12" s="9"/>
+      <c r="L12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="G13" s="26" t="s">
+      <c r="B13" s="10"/>
+      <c r="G13" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27" t="s">
+      <c r="H13" s="24"/>
+      <c r="I13" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="28"/>
+      <c r="J13" s="25"/>
     </row>
     <row r="14" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="30"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="L14" s="16" t="s">
+      <c r="C14" s="24"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="G14" s="9"/>
+      <c r="L14" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21" t="s">
+      <c r="M14" s="12"/>
+      <c r="N14" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="O14" s="22"/>
+      <c r="O14" s="19"/>
     </row>
     <row r="15" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21" t="s">
+      <c r="H15" s="12"/>
+      <c r="I15" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="J15" s="22"/>
-      <c r="L15" s="19" t="s">
+      <c r="J15" s="19"/>
+      <c r="L15" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="E16" s="28"/>
-      <c r="G16" s="18" t="s">
+      <c r="E16" s="25"/>
+      <c r="G16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3" t="s">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J16" s="4"/>
+      <c r="J16" s="3"/>
     </row>
     <row r="17" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3" t="s">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J17" s="4"/>
-      <c r="L17" s="26" t="s">
+      <c r="J17" s="3"/>
+      <c r="L17" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
-      <c r="O17" s="28"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="25"/>
     </row>
     <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21" t="s">
+      <c r="C18" s="12"/>
+      <c r="D18" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="22"/>
-      <c r="G18" s="19" t="s">
+      <c r="E18" s="19"/>
+      <c r="G18" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5" t="s">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="L19" s="26" t="s">
+      <c r="E19" s="3"/>
+      <c r="L19" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="M19" s="27"/>
-      <c r="N19" s="27"/>
-      <c r="O19" s="28"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="25"/>
     </row>
     <row r="20" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
+      <c r="C20" s="2"/>
+      <c r="D20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="4"/>
-      <c r="G20" s="16" t="s">
+      <c r="E20" s="3"/>
+      <c r="G20" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21" t="s">
+      <c r="H20" s="12"/>
+      <c r="I20" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="19" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E21" s="6"/>
-      <c r="G21" s="15" t="s">
+      <c r="E21" s="5"/>
+      <c r="G21" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3" t="s">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L21" s="16" t="s">
+      <c r="L21" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21" t="s">
+      <c r="M21" s="12"/>
+      <c r="N21" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="O21" s="22"/>
+      <c r="O21" s="19"/>
     </row>
     <row r="22" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3" t="s">
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="L22" s="19" t="s">
+      <c r="L22" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5" t="s">
+      <c r="M22" s="4"/>
+      <c r="N22" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="O22" s="6"/>
+      <c r="O22" s="5"/>
     </row>
     <row r="23" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="16" t="s">
+      <c r="B23" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21" t="s">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="22"/>
-      <c r="G23" s="15" t="s">
+      <c r="E23" s="19"/>
+      <c r="G23" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3" t="s">
+      <c r="H23" s="2"/>
+      <c r="I23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="J23" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="G24" s="19" t="s">
+      <c r="E24" s="3"/>
+      <c r="G24" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="6"/>
-      <c r="L24" s="16" t="s">
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="L24" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="19"/>
     </row>
     <row r="25" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3" t="s">
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="E25" s="4"/>
-      <c r="L25" s="19" t="s">
+      <c r="E25" s="3"/>
+      <c r="L25" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="6"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="5"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
+      <c r="C26" s="4"/>
+      <c r="D26" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="E26" s="6"/>
-      <c r="G26" s="17" t="s">
+      <c r="E26" s="5"/>
+      <c r="G26" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21" t="s">
+      <c r="H26" s="12"/>
+      <c r="I26" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="J26" s="22"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3" t="s">
+      <c r="H27" s="2"/>
+      <c r="I27" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J27" s="4"/>
-      <c r="L27" s="16" t="s">
+      <c r="J27" s="3"/>
+      <c r="L27" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-      <c r="O27" s="22"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="19"/>
     </row>
     <row r="28" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16" t="s">
+      <c r="B28" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21" t="s">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="E28" s="22"/>
-      <c r="G28" s="19" t="s">
+      <c r="E28" s="19"/>
+      <c r="G28" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="H28" s="13"/>
-      <c r="I28" s="5" t="s">
+      <c r="H28" s="11"/>
+      <c r="I28" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J28" s="25"/>
-      <c r="L28" s="19" t="s">
+      <c r="J28" s="22"/>
+      <c r="L28" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5" t="s">
+      <c r="M28" s="4"/>
+      <c r="N28" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="O28" s="6"/>
+      <c r="O28" s="5"/>
     </row>
     <row r="29" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="E29" s="4"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E30" s="4"/>
-      <c r="G30" s="16" t="s">
+      <c r="E30" s="3"/>
+      <c r="G30" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
-      <c r="J30" s="22"/>
-      <c r="L30" s="16" t="s">
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="19"/>
+      <c r="L30" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="M30" s="21"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="22"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="19"/>
     </row>
     <row r="31" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5" t="s">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="6"/>
-      <c r="G31" s="19" t="s">
+      <c r="E31" s="5"/>
+      <c r="G31" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="6"/>
-      <c r="L31" s="19" t="s">
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="5"/>
+      <c r="L31" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="6"/>
-    </row>
-    <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-    </row>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21" t="s">
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E33" s="22"/>
-      <c r="G33" s="16" t="s">
+      <c r="E33" s="19"/>
+      <c r="G33" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21" t="s">
+      <c r="H33" s="12"/>
+      <c r="I33" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="J33" s="22"/>
-      <c r="L33" s="16" t="s">
+      <c r="J33" s="19"/>
+      <c r="L33" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="22"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="19"/>
     </row>
     <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3" t="s">
+      <c r="C34" s="2"/>
+      <c r="D34" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E34" s="4"/>
-      <c r="G34" s="19" t="s">
+      <c r="E34" s="3"/>
+      <c r="G34" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
+      <c r="H34" s="4"/>
+      <c r="I34" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J34" s="6"/>
-      <c r="L34" s="19" t="s">
+      <c r="J34" s="5"/>
+      <c r="L34" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="6"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="5"/>
     </row>
     <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3" t="s">
+      <c r="C35" s="2"/>
+      <c r="D35" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E35" s="4"/>
+      <c r="E35" s="3"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3" t="s">
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E36" s="4"/>
-      <c r="L36" s="16" t="s">
+      <c r="E36" s="3"/>
+      <c r="L36" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="M36" s="21"/>
-      <c r="N36" s="21"/>
-      <c r="O36" s="22"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="19"/>
     </row>
     <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="19" t="s">
+      <c r="B37" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="6"/>
-      <c r="L37" s="19" t="s">
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="5"/>
+      <c r="L37" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="6"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="5"/>
     </row>
     <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L39" s="16" t="s">
+      <c r="L39" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="22"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="19"/>
     </row>
     <row r="40" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L40" s="19" t="s">
+      <c r="L40" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="6"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="F79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="F80" s="2"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Update Switch and burron references
Correction to some switches and buttons
</commit_message>
<xml_diff>
--- a/Maps/HOTAS Switch and Button - Quick Reference - BASIC.xlsx
+++ b/Maps/HOTAS Switch and Button - Quick Reference - BASIC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Den\OneDrive\Personal\Thrustmaster\TARGET\Clicker\Development\ED_TargetScript-502\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E077DADF-E796-4176-8124-10692BCFDF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B68721EE-F404-4B68-8B5C-7582CE09B2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12510" yWindow="990" windowWidth="28305" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7545" yWindow="1110" windowWidth="28305" windowHeight="18765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="110">
   <si>
     <t>TG1</t>
   </si>
@@ -297,18 +297,6 @@
     <t>IDLELOFF</t>
   </si>
   <si>
-    <t>Alternate Roll Control (CCW)</t>
-  </si>
-  <si>
-    <t>Alternate Roll Control (CW)</t>
-  </si>
-  <si>
-    <t>Alternate Yaw Control (Left)</t>
-  </si>
-  <si>
-    <t>Alternate Yaw Control (Right)</t>
-  </si>
-  <si>
     <t>Hardpoints</t>
   </si>
   <si>
@@ -346,9 +334,6 @@
   </si>
   <si>
     <t>Forward Thrust</t>
-  </si>
-  <si>
-    <t>(no rudders)</t>
   </si>
   <si>
     <t>Throttle (lever)</t>
@@ -750,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -857,6 +842,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -875,13 +869,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1170,7 +1167,7 @@
   <dimension ref="B1:O40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20:I23"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,43 +1192,43 @@
   <sheetData>
     <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="38"/>
+      <c r="B2" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="41"/>
-      <c r="G4" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="41"/>
-      <c r="L4" s="39" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="44"/>
+      <c r="G4" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
+      <c r="L4" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="40"/>
-      <c r="N4" s="40"/>
-      <c r="O4" s="41"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="44"/>
     </row>
     <row r="5" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
@@ -1334,7 +1331,7 @@
       </c>
       <c r="C10" s="24"/>
       <c r="D10" s="24" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E10" s="25"/>
     </row>
@@ -1353,7 +1350,7 @@
       </c>
       <c r="M11" s="12"/>
       <c r="N11" s="12" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="O11" s="19"/>
     </row>
@@ -1398,7 +1395,7 @@
       </c>
       <c r="M14" s="12"/>
       <c r="N14" s="12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="O14" s="19"/>
     </row>
@@ -1407,7 +1404,7 @@
         <v>35</v>
       </c>
       <c r="H15" s="12"/>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="36" t="s">
         <v>85</v>
       </c>
       <c r="J15" s="19"/>
@@ -1424,14 +1421,14 @@
       </c>
       <c r="C16" s="24"/>
       <c r="D16" s="24" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E16" s="25"/>
       <c r="G16" s="16" t="s">
         <v>36</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="37" t="s">
         <v>86</v>
       </c>
       <c r="J16" s="3"/>
@@ -1441,7 +1438,7 @@
         <v>37</v>
       </c>
       <c r="H17" s="2"/>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="37" t="s">
         <v>73</v>
       </c>
       <c r="J17" s="3"/>
@@ -1465,7 +1462,7 @@
         <v>38</v>
       </c>
       <c r="H18" s="4"/>
-      <c r="I18" s="44" t="s">
+      <c r="I18" s="38" t="s">
         <v>74</v>
       </c>
       <c r="J18" s="5"/>
@@ -1492,19 +1489,15 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E20" s="3"/>
       <c r="G20" s="14" t="s">
         <v>39</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="42" t="s">
-        <v>90</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>107</v>
-      </c>
+      <c r="I20" s="45"/>
+      <c r="J20" s="46"/>
     </row>
     <row r="21" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="17" t="s">
@@ -1512,19 +1505,15 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21" s="13" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="I21" s="47"/>
+      <c r="J21" s="48"/>
       <c r="L21" s="14" t="s">
         <v>61</v>
       </c>
@@ -1539,12 +1528,8 @@
         <v>41</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="I22" s="43" t="s">
-        <v>92</v>
-      </c>
-      <c r="J22" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="I22" s="47"/>
+      <c r="J22" s="48"/>
       <c r="L22" s="17" t="s">
         <v>62</v>
       </c>
@@ -1567,12 +1552,8 @@
         <v>42</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="I23" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="3" t="s">
-        <v>107</v>
-      </c>
+      <c r="I23" s="47"/>
+      <c r="J23" s="48"/>
     </row>
     <row r="24" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
@@ -1580,7 +1561,7 @@
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="E24" s="3"/>
       <c r="G24" s="17" t="s">
@@ -1602,7 +1583,7 @@
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="E25" s="3"/>
       <c r="L25" s="17" t="s">
@@ -1618,7 +1599,7 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26" s="15" t="s">
@@ -1626,7 +1607,7 @@
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="J26" s="19"/>
     </row>
@@ -1636,7 +1617,7 @@
       </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J27" s="3"/>
       <c r="L27" s="14" t="s">
@@ -1652,7 +1633,7 @@
       </c>
       <c r="C28" s="12"/>
       <c r="D28" s="12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E28" s="19"/>
       <c r="G28" s="17" t="s">
@@ -1678,7 +1659,7 @@
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E29" s="3"/>
     </row>
@@ -1688,7 +1669,7 @@
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E30" s="3"/>
       <c r="G30" s="14" t="s">
@@ -1710,7 +1691,7 @@
       </c>
       <c r="C31" s="4"/>
       <c r="D31" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E31" s="5"/>
       <c r="G31" s="17" t="s">
@@ -1733,7 +1714,7 @@
       </c>
       <c r="C33" s="12"/>
       <c r="D33" s="12" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E33" s="19"/>
       <c r="G33" s="14" t="s">
@@ -1757,7 +1738,7 @@
       </c>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E34" s="3"/>
       <c r="G34" s="17" t="s">
@@ -1781,7 +1762,7 @@
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E35" s="3"/>
     </row>
@@ -1791,7 +1772,7 @@
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E36" s="3"/>
       <c r="L36" s="14" t="s">

</xml_diff>